<commit_message>
Initial commit R2016a. Added hyperlinks to model canvas to change subsystem variants.
</commit_message>
<xml_diff>
--- a/Fuel_Consumption/Fuel_Consumption_DATA.xlsx
+++ b/Fuel_Consumption/Fuel_Consumption_DATA.xlsx
@@ -845,4 +845,241 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e7c50fe4-4c86-4d33-a0d3-ad29cfb7378a" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100525B94EEF47D42499A62120CC90E0AB3" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e706cd362d7e41030bb8c72a7c62a9d5">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c85acdc-a394-4ae0-8c72-fb4a95b3d573" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55e2521e7df4d5c11309cefaa7c01562" ns2:_="">
+    <xsd:import namespace="5c85acdc-a394-4ae0-8c72-fb4a95b3d573"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:_dlc_DocId" minOccurs="0"/>
+                <xsd:element ref="ns2:_dlc_DocIdUrl" minOccurs="0"/>
+                <xsd:element ref="ns2:_dlc_DocIdPersistId" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5c85acdc-a394-4ae0-8c72-fb4a95b3d573" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_dlc_DocId" ma:index="8" nillable="true" ma:displayName="Document ID Value" ma:description="The value of the document ID assigned to this item." ma:internalName="_dlc_DocId" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_dlc_DocIdUrl" ma:index="9" nillable="true" ma:displayName="Document ID" ma:description="Permanent link to this document." ma:hidden="true" ma:internalName="_dlc_DocIdUrl" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:URL">
+            <xsd:sequence>
+              <xsd:element name="Url" type="dms:ValidUrl" minOccurs="0" nillable="true"/>
+              <xsd:element name="Description" type="xsd:string" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="_dlc_DocIdPersistId" ma:index="10" nillable="true" ma:displayName="Persist ID" ma:description="Keep ID on add." ma:hidden="true" ma:internalName="_dlc_DocIdPersistId" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="5c85acdc-a394-4ae0-8c72-fb4a95b3d573">FV3TYEPWNNQC-24-75630</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="5c85acdc-a394-4ae0-8c72-fb4a95b3d573">
+      <Url>http://sharepoint/marketing/product/da/physmod/ecl/_layouts/15/DocIdRedir.aspx?ID=FV3TYEPWNNQC-24-75630</Url>
+      <Description>FV3TYEPWNNQC-24-75630</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7736084B-DF4C-4F3E-8AAB-FC9FDC868D27}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B31D2C5B-5463-4226-900B-A297A9DA2A66}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F28D94D-EE32-41B0-9984-CB69D565A8F4}"/>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB845A5D-F6F0-4597-9E54-4982FBD021FD}"/>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7C5997B-6CD7-47B0-B366-B0676F92C2AC}"/>
 </file>
</xml_diff>